<commit_message>
Updates to NGARDv1601 assays
</commit_message>
<xml_diff>
--- a/assay_data/NGARD_assays.xlsx
+++ b/assay_data/NGARD_assays.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4319" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4312" uniqueCount="897">
   <si>
     <t>Assay Name</t>
   </si>
@@ -3640,7 +3640,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3731,6 +3731,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="508">
@@ -14257,10 +14260,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD252"/>
+  <dimension ref="A1:AD251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="I112" sqref="I112"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15919,7 +15922,7 @@
     </row>
     <row r="65" spans="1:17">
       <c r="A65" t="s">
-        <v>388</v>
+        <v>449</v>
       </c>
       <c r="B65" t="s">
         <v>22</v>
@@ -15927,27 +15930,29 @@
       <c r="C65" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="9"/>
+      <c r="D65" s="42" t="s">
+        <v>452</v>
+      </c>
       <c r="I65" s="9" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="J65">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K65" t="s">
+        <v>402</v>
+      </c>
+      <c r="L65" t="s">
         <v>401</v>
       </c>
-      <c r="L65" t="s">
-        <v>402</v>
-      </c>
-      <c r="P65" t="s">
-        <v>525</v>
+      <c r="P65" s="30" t="s">
+        <v>559</v>
       </c>
       <c r="Q65" s="1"/>
     </row>
     <row r="66" spans="1:17">
       <c r="A66" t="s">
-        <v>449</v>
+        <v>633</v>
       </c>
       <c r="B66" t="s">
         <v>22</v>
@@ -15955,29 +15960,29 @@
       <c r="C66" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>452</v>
+      <c r="D66" s="37" t="s">
+        <v>749</v>
       </c>
       <c r="I66" s="9" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="J66">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K66" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L66" t="s">
-        <v>401</v>
-      </c>
-      <c r="P66" s="30" t="s">
+        <v>400</v>
+      </c>
+      <c r="P66" t="s">
         <v>559</v>
       </c>
       <c r="Q66" s="1"/>
     </row>
     <row r="67" spans="1:17">
       <c r="A67" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B67" t="s">
         <v>22</v>
@@ -15986,19 +15991,19 @@
         <v>26</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="J67">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="K67" t="s">
         <v>401</v>
       </c>
       <c r="L67" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P67" t="s">
         <v>559</v>
@@ -16007,7 +16012,7 @@
     </row>
     <row r="68" spans="1:17">
       <c r="A68" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="B68" t="s">
         <v>22</v>
@@ -16015,29 +16020,27 @@
       <c r="C68" t="s">
         <v>26</v>
       </c>
-      <c r="D68" s="37" t="s">
-        <v>750</v>
-      </c>
+      <c r="D68" s="37"/>
       <c r="I68" s="9" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="J68">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="K68" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="L68" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="P68" t="s">
-        <v>559</v>
+        <v>801</v>
       </c>
       <c r="Q68" s="1"/>
     </row>
     <row r="69" spans="1:17">
       <c r="A69" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B69" t="s">
         <v>22</v>
@@ -16045,27 +16048,29 @@
       <c r="C69" t="s">
         <v>26</v>
       </c>
-      <c r="D69" s="37"/>
+      <c r="D69" s="37" t="s">
+        <v>754</v>
+      </c>
       <c r="I69" s="9" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="J69">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K69" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="L69" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="P69" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="Q69" s="1"/>
     </row>
     <row r="70" spans="1:17">
       <c r="A70" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="B70" t="s">
         <v>22</v>
@@ -16074,28 +16079,28 @@
         <v>26</v>
       </c>
       <c r="D70" s="37" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="J70">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K70" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="L70" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P70" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="Q70" s="1"/>
     </row>
     <row r="71" spans="1:17">
       <c r="A71" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="B71" t="s">
         <v>22</v>
@@ -16104,28 +16109,28 @@
         <v>26</v>
       </c>
       <c r="D71" s="37" t="s">
-        <v>752</v>
+        <v>720</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="J71">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K71" t="s">
         <v>402</v>
       </c>
       <c r="L71" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="P71" t="s">
-        <v>799</v>
+        <v>768</v>
       </c>
       <c r="Q71" s="1"/>
     </row>
     <row r="72" spans="1:17">
       <c r="A72" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B72" t="s">
         <v>22</v>
@@ -16134,10 +16139,10 @@
         <v>26</v>
       </c>
       <c r="D72" s="37" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>862</v>
+        <v>846</v>
       </c>
       <c r="J72">
         <v>34</v>
@@ -16149,13 +16154,13 @@
         <v>401</v>
       </c>
       <c r="P72" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="Q72" s="1"/>
     </row>
     <row r="73" spans="1:17">
       <c r="A73" t="s">
-        <v>602</v>
+        <v>637</v>
       </c>
       <c r="B73" t="s">
         <v>22</v>
@@ -16164,79 +16169,70 @@
         <v>26</v>
       </c>
       <c r="D73" s="37" t="s">
-        <v>719</v>
+        <v>753</v>
       </c>
       <c r="I73" s="9" t="s">
-        <v>846</v>
+        <v>863</v>
       </c>
       <c r="J73">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K73" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="L73" t="s">
         <v>401</v>
       </c>
       <c r="P73" t="s">
-        <v>767</v>
+        <v>800</v>
       </c>
       <c r="Q73" s="1"/>
     </row>
     <row r="74" spans="1:17">
       <c r="A74" t="s">
-        <v>637</v>
+        <v>451</v>
       </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C74" t="s">
         <v>26</v>
       </c>
       <c r="D74" s="37" t="s">
-        <v>753</v>
-      </c>
-      <c r="I74" s="9" t="s">
-        <v>863</v>
-      </c>
-      <c r="J74">
-        <v>35</v>
-      </c>
-      <c r="K74" t="s">
-        <v>399</v>
-      </c>
-      <c r="L74" t="s">
-        <v>401</v>
+        <v>453</v>
+      </c>
+      <c r="I74" t="s">
+        <v>843</v>
       </c>
       <c r="P74" t="s">
-        <v>800</v>
+        <v>458</v>
       </c>
       <c r="Q74" s="1"/>
     </row>
     <row r="75" spans="1:17">
       <c r="A75" t="s">
-        <v>451</v>
+        <v>581</v>
       </c>
       <c r="B75" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C75" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D75" s="37" t="s">
-        <v>453</v>
-      </c>
-      <c r="I75" t="s">
-        <v>843</v>
+        <v>662</v>
+      </c>
+      <c r="I75" s="9" t="s">
+        <v>677</v>
       </c>
       <c r="P75" t="s">
-        <v>458</v>
+        <v>826</v>
       </c>
       <c r="Q75" s="1"/>
     </row>
     <row r="76" spans="1:17">
       <c r="A76" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B76" t="s">
         <v>21</v>
@@ -16245,19 +16241,19 @@
         <v>28</v>
       </c>
       <c r="D76" s="37" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I76" s="9" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="P76" t="s">
-        <v>826</v>
+        <v>840</v>
       </c>
       <c r="Q76" s="1"/>
     </row>
     <row r="77" spans="1:17">
       <c r="A77" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B77" t="s">
         <v>21</v>
@@ -16266,10 +16262,10 @@
         <v>28</v>
       </c>
       <c r="D77" s="37" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="I77" s="9" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="P77" t="s">
         <v>840</v>
@@ -16278,7 +16274,7 @@
     </row>
     <row r="78" spans="1:17">
       <c r="A78" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B78" t="s">
         <v>21</v>
@@ -16287,19 +16283,19 @@
         <v>28</v>
       </c>
       <c r="D78" s="37" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="P78" t="s">
-        <v>840</v>
+        <v>827</v>
       </c>
       <c r="Q78" s="1"/>
     </row>
     <row r="79" spans="1:17">
       <c r="A79" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="B79" t="s">
         <v>21</v>
@@ -16308,19 +16304,19 @@
         <v>28</v>
       </c>
       <c r="D79" s="37" t="s">
-        <v>663</v>
+        <v>650</v>
       </c>
       <c r="I79" s="9" t="s">
-        <v>678</v>
+        <v>665</v>
       </c>
       <c r="P79" t="s">
-        <v>827</v>
+        <v>837</v>
       </c>
       <c r="Q79" s="1"/>
     </row>
     <row r="80" spans="1:17">
       <c r="A80" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B80" t="s">
         <v>21</v>
@@ -16329,10 +16325,10 @@
         <v>28</v>
       </c>
       <c r="D80" s="37" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="I80" s="9" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="P80" t="s">
         <v>837</v>
@@ -16341,7 +16337,7 @@
     </row>
     <row r="81" spans="1:17">
       <c r="A81" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B81" t="s">
         <v>21</v>
@@ -16350,10 +16346,10 @@
         <v>28</v>
       </c>
       <c r="D81" s="37" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="I81" s="9" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="P81" t="s">
         <v>837</v>
@@ -16362,7 +16358,7 @@
     </row>
     <row r="82" spans="1:17">
       <c r="A82" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B82" t="s">
         <v>21</v>
@@ -16371,10 +16367,10 @@
         <v>28</v>
       </c>
       <c r="D82" s="37" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="P82" t="s">
         <v>837</v>
@@ -16383,7 +16379,7 @@
     </row>
     <row r="83" spans="1:17">
       <c r="A83" t="s">
-        <v>572</v>
+        <v>583</v>
       </c>
       <c r="B83" t="s">
         <v>21</v>
@@ -16392,19 +16388,19 @@
         <v>28</v>
       </c>
       <c r="D83" s="37" t="s">
-        <v>652</v>
+        <v>664</v>
       </c>
       <c r="I83" s="9" t="s">
-        <v>668</v>
+        <v>679</v>
       </c>
       <c r="P83" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
       <c r="Q83" s="1"/>
     </row>
     <row r="84" spans="1:17">
       <c r="A84" t="s">
-        <v>583</v>
+        <v>573</v>
       </c>
       <c r="B84" t="s">
         <v>21</v>
@@ -16413,19 +16409,19 @@
         <v>28</v>
       </c>
       <c r="D84" s="37" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="I84" s="9" t="s">
-        <v>679</v>
+        <v>669</v>
       </c>
       <c r="P84" t="s">
-        <v>828</v>
+        <v>838</v>
       </c>
       <c r="Q84" s="1"/>
     </row>
     <row r="85" spans="1:17">
       <c r="A85" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B85" t="s">
         <v>21</v>
@@ -16434,19 +16430,19 @@
         <v>28</v>
       </c>
       <c r="D85" s="37" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="I85" s="9" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="P85" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="Q85" s="1"/>
     </row>
     <row r="86" spans="1:17">
       <c r="A86" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B86" t="s">
         <v>21</v>
@@ -16455,10 +16451,10 @@
         <v>28</v>
       </c>
       <c r="D86" s="37" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="I86" s="9" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="P86" t="s">
         <v>839</v>
@@ -16467,7 +16463,7 @@
     </row>
     <row r="87" spans="1:17">
       <c r="A87" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B87" t="s">
         <v>21</v>
@@ -16476,10 +16472,10 @@
         <v>28</v>
       </c>
       <c r="D87" s="37" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="I87" s="9" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="P87" t="s">
         <v>839</v>
@@ -16488,7 +16484,7 @@
     </row>
     <row r="88" spans="1:17">
       <c r="A88" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B88" t="s">
         <v>21</v>
@@ -16497,10 +16493,10 @@
         <v>28</v>
       </c>
       <c r="D88" s="37" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="I88" s="9" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="P88" t="s">
         <v>839</v>
@@ -16509,41 +16505,37 @@
     </row>
     <row r="89" spans="1:17">
       <c r="A89" t="s">
-        <v>578</v>
+        <v>641</v>
       </c>
       <c r="B89" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
-      </c>
-      <c r="D89" s="37" t="s">
-        <v>659</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D89" s="37"/>
       <c r="I89" s="9" t="s">
-        <v>674</v>
+        <v>700</v>
+      </c>
+      <c r="J89">
+        <v>39</v>
+      </c>
+      <c r="K89" t="s">
+        <v>400</v>
+      </c>
+      <c r="L89" t="s">
+        <v>399</v>
       </c>
       <c r="P89" t="s">
-        <v>839</v>
+        <v>766</v>
       </c>
       <c r="Q89" s="1"/>
     </row>
     <row r="90" spans="1:17">
-      <c r="A90" t="s">
-        <v>641</v>
-      </c>
-      <c r="B90" t="s">
-        <v>22</v>
-      </c>
-      <c r="C90" t="s">
-        <v>25</v>
-      </c>
       <c r="D90" s="37"/>
-      <c r="I90" s="9" t="s">
-        <v>700</v>
-      </c>
+      <c r="I90" s="9"/>
       <c r="J90">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="K90" t="s">
         <v>400</v>
@@ -16560,13 +16552,13 @@
       <c r="D91" s="37"/>
       <c r="I91" s="9"/>
       <c r="J91">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="K91" t="s">
+        <v>399</v>
+      </c>
+      <c r="L91" t="s">
         <v>400</v>
-      </c>
-      <c r="L91" t="s">
-        <v>399</v>
       </c>
       <c r="P91" t="s">
         <v>766</v>
@@ -16577,13 +16569,13 @@
       <c r="D92" s="37"/>
       <c r="I92" s="9"/>
       <c r="J92">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="K92" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="L92" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="P92" t="s">
         <v>766</v>
@@ -16594,10 +16586,10 @@
       <c r="D93" s="37"/>
       <c r="I93" s="9"/>
       <c r="J93">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="K93" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L93" t="s">
         <v>402</v>
@@ -16611,10 +16603,10 @@
       <c r="D94" s="37"/>
       <c r="I94" s="9"/>
       <c r="J94">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="K94" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="L94" t="s">
         <v>402</v>
@@ -16625,46 +16617,46 @@
       <c r="Q94" s="1"/>
     </row>
     <row r="95" spans="1:17">
-      <c r="D95" s="37"/>
-      <c r="I95" s="9"/>
+      <c r="A95" t="s">
+        <v>640</v>
+      </c>
+      <c r="B95" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" t="s">
+        <v>25</v>
+      </c>
+      <c r="D95" s="37" t="s">
+        <v>755</v>
+      </c>
+      <c r="I95" s="9" t="s">
+        <v>699</v>
+      </c>
       <c r="J95">
-        <v>147</v>
+        <v>43</v>
       </c>
       <c r="K95" t="s">
         <v>401</v>
       </c>
       <c r="L95" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="P95" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="Q95" s="1"/>
     </row>
     <row r="96" spans="1:17">
-      <c r="A96" t="s">
-        <v>640</v>
-      </c>
-      <c r="B96" t="s">
-        <v>22</v>
-      </c>
-      <c r="C96" t="s">
-        <v>25</v>
-      </c>
-      <c r="D96" s="37" t="s">
-        <v>755</v>
-      </c>
-      <c r="I96" s="9" t="s">
-        <v>699</v>
-      </c>
+      <c r="D96" s="37"/>
+      <c r="I96" s="9"/>
       <c r="J96">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="K96" t="s">
         <v>401</v>
       </c>
       <c r="L96" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="P96" t="s">
         <v>765</v>
@@ -16675,13 +16667,13 @@
       <c r="D97" s="37"/>
       <c r="I97" s="9"/>
       <c r="J97">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="K97" t="s">
+        <v>402</v>
+      </c>
+      <c r="L97" t="s">
         <v>401</v>
-      </c>
-      <c r="L97" t="s">
-        <v>402</v>
       </c>
       <c r="P97" t="s">
         <v>765</v>
@@ -16692,13 +16684,13 @@
       <c r="D98" s="37"/>
       <c r="I98" s="9"/>
       <c r="J98">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="K98" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="L98" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P98" t="s">
         <v>765</v>
@@ -16709,13 +16701,13 @@
       <c r="D99" s="37"/>
       <c r="I99" s="9"/>
       <c r="J99">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="K99" t="s">
         <v>399</v>
       </c>
       <c r="L99" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="P99" t="s">
         <v>765</v>
@@ -16726,13 +16718,13 @@
       <c r="D100" s="37"/>
       <c r="I100" s="9"/>
       <c r="J100">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="K100" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="L100" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="P100" t="s">
         <v>765</v>
@@ -16743,13 +16735,13 @@
       <c r="D101" s="37"/>
       <c r="I101" s="9"/>
       <c r="J101">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K101" t="s">
+        <v>399</v>
+      </c>
+      <c r="L101" t="s">
         <v>401</v>
-      </c>
-      <c r="L101" t="s">
-        <v>402</v>
       </c>
       <c r="P101" t="s">
         <v>765</v>
@@ -16760,13 +16752,13 @@
       <c r="D102" s="37"/>
       <c r="I102" s="9"/>
       <c r="J102">
-        <v>184</v>
+        <v>220</v>
       </c>
       <c r="K102" t="s">
+        <v>400</v>
+      </c>
+      <c r="L102" t="s">
         <v>399</v>
-      </c>
-      <c r="L102" t="s">
-        <v>401</v>
       </c>
       <c r="P102" t="s">
         <v>765</v>
@@ -16777,7 +16769,7 @@
       <c r="D103" s="37"/>
       <c r="I103" s="9"/>
       <c r="J103">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="K103" t="s">
         <v>400</v>
@@ -16791,25 +16783,28 @@
       <c r="Q103" s="1"/>
     </row>
     <row r="104" spans="1:17">
-      <c r="D104" s="37"/>
-      <c r="I104" s="9"/>
-      <c r="J104">
-        <v>235</v>
-      </c>
-      <c r="K104" t="s">
-        <v>400</v>
-      </c>
-      <c r="L104" t="s">
-        <v>399</v>
+      <c r="A104" t="s">
+        <v>36</v>
+      </c>
+      <c r="B104" t="s">
+        <v>21</v>
+      </c>
+      <c r="C104" t="s">
+        <v>25</v>
+      </c>
+      <c r="D104" t="s">
+        <v>52</v>
+      </c>
+      <c r="I104" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="P104" t="s">
-        <v>765</v>
-      </c>
-      <c r="Q104" s="1"/>
+        <v>499</v>
+      </c>
     </row>
     <row r="105" spans="1:17">
       <c r="A105" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B105" t="s">
         <v>21</v>
@@ -16817,19 +16812,16 @@
       <c r="C105" t="s">
         <v>25</v>
       </c>
-      <c r="D105" t="s">
-        <v>52</v>
-      </c>
       <c r="I105" s="9" t="s">
-        <v>37</v>
+        <v>463</v>
       </c>
       <c r="P105" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="106" spans="1:17">
       <c r="A106" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B106" t="s">
         <v>21</v>
@@ -16838,15 +16830,15 @@
         <v>25</v>
       </c>
       <c r="I106" s="9" t="s">
-        <v>463</v>
+        <v>40</v>
       </c>
       <c r="P106" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="107" spans="1:17">
       <c r="A107" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B107" t="s">
         <v>21</v>
@@ -16855,15 +16847,15 @@
         <v>25</v>
       </c>
       <c r="I107" s="9" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="P107" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
     </row>
     <row r="108" spans="1:17">
       <c r="A108" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B108" t="s">
         <v>21</v>
@@ -16871,8 +16863,11 @@
       <c r="C108" t="s">
         <v>25</v>
       </c>
+      <c r="D108" t="s">
+        <v>59</v>
+      </c>
       <c r="I108" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P108" t="s">
         <v>505</v>
@@ -16880,7 +16875,7 @@
     </row>
     <row r="109" spans="1:17">
       <c r="A109" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B109" t="s">
         <v>21</v>
@@ -16889,90 +16884,81 @@
         <v>25</v>
       </c>
       <c r="D109" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="I109" s="9" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="P109" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="110" spans="1:17">
       <c r="A110" t="s">
-        <v>33</v>
+        <v>895</v>
       </c>
       <c r="B110" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C110" t="s">
         <v>25</v>
       </c>
       <c r="D110" t="s">
-        <v>35</v>
-      </c>
-      <c r="I110" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="P110" t="s">
-        <v>498</v>
+        <v>461</v>
+      </c>
+      <c r="I110" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="111" spans="1:17">
       <c r="A111" t="s">
-        <v>895</v>
+        <v>68</v>
       </c>
       <c r="B111" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C111" t="s">
         <v>25</v>
       </c>
       <c r="D111" t="s">
-        <v>461</v>
-      </c>
-      <c r="I111" t="s">
-        <v>896</v>
+        <v>71</v>
+      </c>
+      <c r="I111" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P111" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="112" spans="1:17">
       <c r="A112" t="s">
-        <v>68</v>
+        <v>358</v>
       </c>
       <c r="B112" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C112" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D112" t="s">
-        <v>71</v>
+        <v>359</v>
+      </c>
+      <c r="H112" t="s">
+        <v>368</v>
       </c>
       <c r="I112" s="9" t="s">
-        <v>65</v>
+        <v>360</v>
       </c>
       <c r="P112" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
     </row>
     <row r="113" spans="1:16">
-      <c r="A113" t="s">
-        <v>358</v>
-      </c>
-      <c r="B113" t="s">
-        <v>23</v>
-      </c>
-      <c r="C113" t="s">
-        <v>26</v>
-      </c>
-      <c r="D113" t="s">
-        <v>359</v>
-      </c>
       <c r="H113" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I113" s="9" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="P113" t="s">
         <v>518</v>
@@ -16980,10 +16966,10 @@
     </row>
     <row r="114" spans="1:16">
       <c r="H114" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="I114" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="P114" t="s">
         <v>518</v>
@@ -16991,10 +16977,10 @@
     </row>
     <row r="115" spans="1:16">
       <c r="H115" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="I115" s="9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="P115" t="s">
         <v>518</v>
@@ -17002,52 +16988,61 @@
     </row>
     <row r="116" spans="1:16">
       <c r="H116" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="I116" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="P116" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="117" spans="1:16">
+      <c r="A117" t="s">
+        <v>366</v>
+      </c>
+      <c r="B117" t="s">
+        <v>23</v>
+      </c>
+      <c r="C117" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117" t="s">
+        <v>367</v>
+      </c>
       <c r="H117" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="I117" s="9" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="P117" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="118" spans="1:16">
       <c r="A118" t="s">
-        <v>366</v>
+        <v>476</v>
       </c>
       <c r="B118" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C118" t="s">
         <v>26</v>
       </c>
       <c r="D118" t="s">
-        <v>367</v>
-      </c>
-      <c r="H118" t="s">
-        <v>373</v>
+        <v>486</v>
       </c>
       <c r="I118" s="9" t="s">
-        <v>365</v>
+        <v>491</v>
       </c>
       <c r="P118" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
     </row>
     <row r="119" spans="1:16">
       <c r="A119" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B119" t="s">
         <v>21</v>
@@ -17059,15 +17054,15 @@
         <v>486</v>
       </c>
       <c r="I119" s="9" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="P119" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="120" spans="1:16">
       <c r="A120" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B120" t="s">
         <v>21</v>
@@ -17079,15 +17074,15 @@
         <v>486</v>
       </c>
       <c r="I120" s="9" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="P120" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="121" spans="1:16">
       <c r="A121" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B121" t="s">
         <v>21</v>
@@ -17099,15 +17094,15 @@
         <v>486</v>
       </c>
       <c r="I121" s="9" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="P121" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="122" spans="1:16">
       <c r="A122" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B122" t="s">
         <v>21</v>
@@ -17119,15 +17114,15 @@
         <v>486</v>
       </c>
       <c r="I122" s="9" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="P122" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="123" spans="1:16">
       <c r="A123" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B123" t="s">
         <v>21</v>
@@ -17139,15 +17134,15 @@
         <v>486</v>
       </c>
       <c r="I123" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="P123" t="s">
-        <v>533</v>
+        <v>489</v>
+      </c>
+      <c r="P123" s="14" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="124" spans="1:16">
       <c r="A124" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B124" t="s">
         <v>21</v>
@@ -17159,15 +17154,15 @@
         <v>486</v>
       </c>
       <c r="I124" s="9" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="P124" s="14" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="125" spans="1:16">
       <c r="A125" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B125" t="s">
         <v>21</v>
@@ -17179,15 +17174,15 @@
         <v>486</v>
       </c>
       <c r="I125" s="9" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="P125" s="14" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="126" spans="1:16">
       <c r="A126" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B126" t="s">
         <v>21</v>
@@ -17199,15 +17194,15 @@
         <v>486</v>
       </c>
       <c r="I126" s="9" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="P126" s="14" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="127" spans="1:16">
       <c r="A127" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B127" t="s">
         <v>21</v>
@@ -17219,7 +17214,7 @@
         <v>486</v>
       </c>
       <c r="I127" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="P127" s="14" t="s">
         <v>537</v>
@@ -17227,27 +17222,36 @@
     </row>
     <row r="128" spans="1:16">
       <c r="A128" t="s">
-        <v>485</v>
+        <v>389</v>
       </c>
       <c r="B128" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C128" t="s">
         <v>26</v>
       </c>
       <c r="D128" t="s">
-        <v>486</v>
+        <v>398</v>
       </c>
       <c r="I128" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="P128" s="14" t="s">
-        <v>537</v>
+        <v>396</v>
+      </c>
+      <c r="J128">
+        <v>30</v>
+      </c>
+      <c r="K128" t="s">
+        <v>402</v>
+      </c>
+      <c r="L128" t="s">
+        <v>401</v>
+      </c>
+      <c r="P128" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="129" spans="1:17">
       <c r="A129" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B129" t="s">
         <v>22</v>
@@ -17256,27 +17260,27 @@
         <v>26</v>
       </c>
       <c r="D129" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I129" s="9" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="J129">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="K129" t="s">
+        <v>401</v>
+      </c>
+      <c r="L129" t="s">
         <v>402</v>
       </c>
-      <c r="L129" t="s">
-        <v>401</v>
-      </c>
       <c r="P129" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="130" spans="1:17">
       <c r="A130" t="s">
-        <v>384</v>
+        <v>822</v>
       </c>
       <c r="B130" t="s">
         <v>22</v>
@@ -17284,28 +17288,26 @@
       <c r="C130" t="s">
         <v>26</v>
       </c>
-      <c r="D130" t="s">
-        <v>397</v>
-      </c>
       <c r="I130" s="9" t="s">
-        <v>391</v>
+        <v>821</v>
       </c>
       <c r="J130">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="K130" t="s">
+        <v>402</v>
+      </c>
+      <c r="L130" t="s">
         <v>401</v>
       </c>
-      <c r="L130" t="s">
-        <v>402</v>
-      </c>
       <c r="P130" t="s">
-        <v>521</v>
-      </c>
+        <v>823</v>
+      </c>
+      <c r="Q130" s="1"/>
     </row>
     <row r="131" spans="1:17">
       <c r="A131" t="s">
-        <v>822</v>
+        <v>388</v>
       </c>
       <c r="B131" t="s">
         <v>22</v>
@@ -17314,25 +17316,24 @@
         <v>26</v>
       </c>
       <c r="I131" s="9" t="s">
-        <v>821</v>
+        <v>395</v>
       </c>
       <c r="J131">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="K131" t="s">
+        <v>401</v>
+      </c>
+      <c r="L131" t="s">
         <v>402</v>
       </c>
-      <c r="L131" t="s">
-        <v>401</v>
-      </c>
       <c r="P131" t="s">
-        <v>823</v>
-      </c>
-      <c r="Q131" s="1"/>
+        <v>525</v>
+      </c>
     </row>
     <row r="132" spans="1:17">
       <c r="A132" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B132" t="s">
         <v>22</v>
@@ -17341,10 +17342,10 @@
         <v>26</v>
       </c>
       <c r="I132" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J132">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="K132" t="s">
         <v>401</v>
@@ -17353,12 +17354,12 @@
         <v>402</v>
       </c>
       <c r="P132" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="133" spans="1:17">
       <c r="A133" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B133" t="s">
         <v>22</v>
@@ -17367,24 +17368,24 @@
         <v>26</v>
       </c>
       <c r="I133" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="J133">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="K133" t="s">
+        <v>402</v>
+      </c>
+      <c r="L133" t="s">
         <v>401</v>
       </c>
-      <c r="L133" t="s">
-        <v>402</v>
-      </c>
       <c r="P133" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="134" spans="1:17">
       <c r="A134" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B134" t="s">
         <v>22</v>
@@ -17393,24 +17394,24 @@
         <v>26</v>
       </c>
       <c r="I134" s="9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J134">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="K134" t="s">
+        <v>401</v>
+      </c>
+      <c r="L134" t="s">
         <v>402</v>
       </c>
-      <c r="L134" t="s">
-        <v>401</v>
-      </c>
       <c r="P134" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="135" spans="1:17">
       <c r="A135" t="s">
-        <v>385</v>
+        <v>817</v>
       </c>
       <c r="B135" t="s">
         <v>22</v>
@@ -17418,25 +17419,26 @@
       <c r="C135" t="s">
         <v>26</v>
       </c>
-      <c r="I135" s="9" t="s">
-        <v>392</v>
+      <c r="I135" s="26" t="s">
+        <v>819</v>
       </c>
       <c r="J135">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="K135" t="s">
+        <v>400</v>
+      </c>
+      <c r="L135" t="s">
         <v>401</v>
       </c>
-      <c r="L135" t="s">
-        <v>402</v>
-      </c>
       <c r="P135" t="s">
-        <v>522</v>
-      </c>
+        <v>520</v>
+      </c>
+      <c r="Q135" s="1"/>
     </row>
     <row r="136" spans="1:17">
       <c r="A136" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B136" t="s">
         <v>22</v>
@@ -17445,13 +17447,13 @@
         <v>26</v>
       </c>
       <c r="I136" s="26" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="J136">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="K136" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="L136" t="s">
         <v>401</v>
@@ -17463,34 +17465,27 @@
     </row>
     <row r="137" spans="1:17">
       <c r="A137" t="s">
-        <v>818</v>
+        <v>403</v>
       </c>
       <c r="B137" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C137" t="s">
-        <v>26</v>
-      </c>
-      <c r="I137" s="26" t="s">
-        <v>820</v>
-      </c>
-      <c r="J137">
-        <v>46</v>
-      </c>
-      <c r="K137" t="s">
-        <v>402</v>
-      </c>
-      <c r="L137" t="s">
-        <v>401</v>
-      </c>
-      <c r="P137" t="s">
-        <v>520</v>
-      </c>
-      <c r="Q137" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="D137" t="s">
+        <v>405</v>
+      </c>
+      <c r="I137" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="P137" s="17" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="138" spans="1:17">
       <c r="A138" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B138" t="s">
         <v>21</v>
@@ -17499,38 +17494,38 @@
         <v>28</v>
       </c>
       <c r="D138" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I138" s="9" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="P138" s="17" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="139" spans="1:17">
       <c r="A139" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B139" t="s">
         <v>21</v>
       </c>
       <c r="C139" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D139" t="s">
-        <v>406</v>
+        <v>102</v>
       </c>
       <c r="I139" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="P139" s="17" t="s">
-        <v>528</v>
+        <v>108</v>
+      </c>
+      <c r="P139" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="140" spans="1:17">
       <c r="A140" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B140" t="s">
         <v>21</v>
@@ -17539,10 +17534,10 @@
         <v>25</v>
       </c>
       <c r="D140" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I140" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P140" t="s">
         <v>511</v>
@@ -17550,7 +17545,7 @@
     </row>
     <row r="141" spans="1:17">
       <c r="A141" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="B141" t="s">
         <v>21</v>
@@ -17559,18 +17554,18 @@
         <v>25</v>
       </c>
       <c r="D141" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="I141" s="9" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="P141" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="142" spans="1:17">
       <c r="A142" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B142" t="s">
         <v>21</v>
@@ -17579,18 +17574,18 @@
         <v>25</v>
       </c>
       <c r="D142" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I142" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="P142" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="143" spans="1:17">
       <c r="A143" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B143" t="s">
         <v>21</v>
@@ -17599,10 +17594,10 @@
         <v>25</v>
       </c>
       <c r="D143" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I143" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P143" t="s">
         <v>515</v>
@@ -17610,7 +17605,7 @@
     </row>
     <row r="144" spans="1:17">
       <c r="A144" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="B144" t="s">
         <v>21</v>
@@ -17619,18 +17614,18 @@
         <v>25</v>
       </c>
       <c r="D144" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="I144" s="9" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="P144" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="145" spans="1:17">
       <c r="A145" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B145" t="s">
         <v>21</v>
@@ -17639,10 +17634,10 @@
         <v>25</v>
       </c>
       <c r="D145" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I145" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P145" t="s">
         <v>510</v>
@@ -17650,7 +17645,7 @@
     </row>
     <row r="146" spans="1:17">
       <c r="A146" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B146" t="s">
         <v>21</v>
@@ -17659,58 +17654,58 @@
         <v>25</v>
       </c>
       <c r="D146" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="I146" s="9" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="P146" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="147" spans="1:17">
       <c r="A147" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B147" t="s">
         <v>21</v>
       </c>
       <c r="C147" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D147" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I147" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P147" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="148" spans="1:17">
       <c r="A148" t="s">
-        <v>120</v>
+        <v>329</v>
       </c>
       <c r="B148" t="s">
         <v>21</v>
       </c>
       <c r="C148" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D148" t="s">
-        <v>132</v>
+        <v>339</v>
       </c>
       <c r="I148" s="9" t="s">
-        <v>126</v>
+        <v>349</v>
       </c>
       <c r="P148" t="s">
-        <v>513</v>
+        <v>160</v>
       </c>
     </row>
     <row r="149" spans="1:17">
       <c r="A149" t="s">
-        <v>329</v>
+        <v>589</v>
       </c>
       <c r="B149" t="s">
         <v>21</v>
@@ -17718,19 +17713,20 @@
       <c r="C149" t="s">
         <v>27</v>
       </c>
-      <c r="D149" t="s">
-        <v>339</v>
+      <c r="D149" s="37" t="s">
+        <v>712</v>
       </c>
       <c r="I149" s="9" t="s">
-        <v>349</v>
+        <v>685</v>
       </c>
       <c r="P149" t="s">
         <v>160</v>
       </c>
+      <c r="Q149" s="1"/>
     </row>
     <row r="150" spans="1:17">
       <c r="A150" t="s">
-        <v>589</v>
+        <v>156</v>
       </c>
       <c r="B150" t="s">
         <v>21</v>
@@ -17738,20 +17734,19 @@
       <c r="C150" t="s">
         <v>27</v>
       </c>
-      <c r="D150" s="37" t="s">
-        <v>712</v>
-      </c>
-      <c r="I150" s="9" t="s">
-        <v>685</v>
+      <c r="D150" t="s">
+        <v>159</v>
+      </c>
+      <c r="I150" s="11" t="s">
+        <v>467</v>
       </c>
       <c r="P150" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q150" s="1"/>
+        <v>516</v>
+      </c>
     </row>
     <row r="151" spans="1:17">
       <c r="A151" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B151" t="s">
         <v>21</v>
@@ -17763,7 +17758,7 @@
         <v>159</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P151" t="s">
         <v>516</v>
@@ -17771,7 +17766,7 @@
     </row>
     <row r="152" spans="1:17">
       <c r="A152" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B152" t="s">
         <v>21</v>
@@ -17782,8 +17777,8 @@
       <c r="D152" t="s">
         <v>159</v>
       </c>
-      <c r="I152" s="11" t="s">
-        <v>466</v>
+      <c r="I152" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="P152" t="s">
         <v>516</v>
@@ -17791,7 +17786,7 @@
     </row>
     <row r="153" spans="1:17">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B153" t="s">
         <v>21</v>
@@ -17803,7 +17798,7 @@
         <v>159</v>
       </c>
       <c r="I153" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="P153" t="s">
         <v>516</v>
@@ -17811,7 +17806,7 @@
     </row>
     <row r="154" spans="1:17">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B154" t="s">
         <v>21</v>
@@ -17822,8 +17817,8 @@
       <c r="D154" t="s">
         <v>159</v>
       </c>
-      <c r="I154" s="9" t="s">
-        <v>158</v>
+      <c r="I154" s="11" t="s">
+        <v>464</v>
       </c>
       <c r="P154" t="s">
         <v>516</v>
@@ -17831,7 +17826,7 @@
     </row>
     <row r="155" spans="1:17">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B155" t="s">
         <v>21</v>
@@ -17843,7 +17838,7 @@
         <v>159</v>
       </c>
       <c r="I155" s="11" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="P155" t="s">
         <v>516</v>
@@ -17851,7 +17846,7 @@
     </row>
     <row r="156" spans="1:17">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>330</v>
       </c>
       <c r="B156" t="s">
         <v>21</v>
@@ -17860,18 +17855,18 @@
         <v>27</v>
       </c>
       <c r="D156" t="s">
-        <v>159</v>
-      </c>
-      <c r="I156" s="11" t="s">
-        <v>465</v>
+        <v>340</v>
+      </c>
+      <c r="I156" s="9" t="s">
+        <v>350</v>
       </c>
       <c r="P156" t="s">
-        <v>516</v>
+        <v>550</v>
       </c>
     </row>
     <row r="157" spans="1:17">
       <c r="A157" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B157" t="s">
         <v>21</v>
@@ -17880,18 +17875,18 @@
         <v>27</v>
       </c>
       <c r="D157" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I157" s="9" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="P157" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="158" spans="1:17">
       <c r="A158" t="s">
-        <v>327</v>
+        <v>141</v>
       </c>
       <c r="B158" t="s">
         <v>21</v>
@@ -17900,18 +17895,18 @@
         <v>27</v>
       </c>
       <c r="D158" t="s">
-        <v>337</v>
+        <v>145</v>
       </c>
       <c r="I158" s="9" t="s">
-        <v>347</v>
+        <v>143</v>
       </c>
       <c r="P158" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="159" spans="1:17">
       <c r="A159" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B159" t="s">
         <v>21</v>
@@ -17923,15 +17918,16 @@
         <v>145</v>
       </c>
       <c r="I159" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="P159" t="s">
         <v>551</v>
       </c>
+      <c r="Q159" s="1"/>
     </row>
     <row r="160" spans="1:17">
       <c r="A160" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B160" t="s">
         <v>21</v>
@@ -17940,19 +17936,18 @@
         <v>27</v>
       </c>
       <c r="D160" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="I160" s="9" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="P160" t="s">
-        <v>551</v>
-      </c>
-      <c r="Q160" s="1"/>
+        <v>552</v>
+      </c>
     </row>
     <row r="161" spans="1:17">
       <c r="A161" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B161" t="s">
         <v>21</v>
@@ -17964,15 +17959,16 @@
         <v>148</v>
       </c>
       <c r="I161" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="P161" t="s">
         <v>552</v>
       </c>
+      <c r="Q161" s="1"/>
     </row>
     <row r="162" spans="1:17">
       <c r="A162" t="s">
-        <v>147</v>
+        <v>236</v>
       </c>
       <c r="B162" t="s">
         <v>21</v>
@@ -17981,19 +17977,18 @@
         <v>27</v>
       </c>
       <c r="D162" t="s">
-        <v>148</v>
+        <v>241</v>
       </c>
       <c r="I162" s="9" t="s">
-        <v>150</v>
+        <v>243</v>
       </c>
       <c r="P162" t="s">
-        <v>552</v>
-      </c>
-      <c r="Q162" s="1"/>
+        <v>538</v>
+      </c>
     </row>
     <row r="163" spans="1:17">
       <c r="A163" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B163" t="s">
         <v>21</v>
@@ -18005,7 +18000,7 @@
         <v>241</v>
       </c>
       <c r="I163" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P163" t="s">
         <v>538</v>
@@ -18013,7 +18008,7 @@
     </row>
     <row r="164" spans="1:17">
       <c r="A164" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B164" t="s">
         <v>21</v>
@@ -18025,7 +18020,7 @@
         <v>241</v>
       </c>
       <c r="I164" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="P164" t="s">
         <v>538</v>
@@ -18033,7 +18028,7 @@
     </row>
     <row r="165" spans="1:17">
       <c r="A165" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B165" t="s">
         <v>21</v>
@@ -18045,15 +18040,16 @@
         <v>241</v>
       </c>
       <c r="I165" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="P165" t="s">
         <v>538</v>
       </c>
+      <c r="Q165" s="1"/>
     </row>
     <row r="166" spans="1:17">
       <c r="A166" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B166" t="s">
         <v>21</v>
@@ -18065,16 +18061,15 @@
         <v>241</v>
       </c>
       <c r="I166" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="P166" t="s">
         <v>538</v>
       </c>
-      <c r="Q166" s="1"/>
     </row>
     <row r="167" spans="1:17">
       <c r="A167" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B167" t="s">
         <v>21</v>
@@ -18086,15 +18081,16 @@
         <v>241</v>
       </c>
       <c r="I167" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="P167" t="s">
         <v>538</v>
       </c>
+      <c r="Q167" s="1"/>
     </row>
     <row r="168" spans="1:17">
       <c r="A168" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B168" t="s">
         <v>21</v>
@@ -18106,16 +18102,15 @@
         <v>241</v>
       </c>
       <c r="I168" s="9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P168" t="s">
         <v>538</v>
       </c>
-      <c r="Q168" s="1"/>
     </row>
     <row r="169" spans="1:17">
       <c r="A169" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B169" t="s">
         <v>21</v>
@@ -18127,15 +18122,16 @@
         <v>241</v>
       </c>
       <c r="I169" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="P169" t="s">
         <v>538</v>
       </c>
+      <c r="Q169" s="1"/>
     </row>
     <row r="170" spans="1:17">
       <c r="A170" t="s">
-        <v>240</v>
+        <v>591</v>
       </c>
       <c r="B170" t="s">
         <v>21</v>
@@ -18143,20 +18139,20 @@
       <c r="C170" t="s">
         <v>27</v>
       </c>
-      <c r="D170" t="s">
-        <v>241</v>
+      <c r="D170" s="37" t="s">
+        <v>713</v>
       </c>
       <c r="I170" s="9" t="s">
-        <v>249</v>
+        <v>687</v>
       </c>
       <c r="P170" t="s">
-        <v>538</v>
+        <v>756</v>
       </c>
       <c r="Q170" s="1"/>
     </row>
     <row r="171" spans="1:17">
       <c r="A171" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B171" t="s">
         <v>21</v>
@@ -18165,10 +18161,10 @@
         <v>27</v>
       </c>
       <c r="D171" s="37" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="I171" s="9" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="P171" t="s">
         <v>756</v>
@@ -18177,7 +18173,7 @@
     </row>
     <row r="172" spans="1:17">
       <c r="A172" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B172" t="s">
         <v>21</v>
@@ -18186,10 +18182,10 @@
         <v>27</v>
       </c>
       <c r="D172" s="37" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="I172" s="9" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="P172" t="s">
         <v>756</v>
@@ -18198,7 +18194,7 @@
     </row>
     <row r="173" spans="1:17">
       <c r="A173" t="s">
-        <v>593</v>
+        <v>326</v>
       </c>
       <c r="B173" t="s">
         <v>21</v>
@@ -18206,20 +18202,19 @@
       <c r="C173" t="s">
         <v>27</v>
       </c>
-      <c r="D173" s="37" t="s">
-        <v>715</v>
+      <c r="D173" t="s">
+        <v>336</v>
       </c>
       <c r="I173" s="9" t="s">
-        <v>689</v>
+        <v>346</v>
       </c>
       <c r="P173" t="s">
-        <v>756</v>
-      </c>
-      <c r="Q173" s="1"/>
+        <v>548</v>
+      </c>
     </row>
     <row r="174" spans="1:17">
       <c r="A174" t="s">
-        <v>326</v>
+        <v>597</v>
       </c>
       <c r="B174" t="s">
         <v>21</v>
@@ -18227,40 +18222,49 @@
       <c r="C174" t="s">
         <v>27</v>
       </c>
-      <c r="D174" t="s">
-        <v>336</v>
+      <c r="D174" s="37" t="s">
+        <v>758</v>
       </c>
       <c r="I174" s="9" t="s">
-        <v>346</v>
+        <v>693</v>
       </c>
       <c r="P174" t="s">
-        <v>548</v>
-      </c>
+        <v>764</v>
+      </c>
+      <c r="Q174" s="1"/>
     </row>
     <row r="175" spans="1:17">
       <c r="A175" t="s">
-        <v>597</v>
+        <v>166</v>
       </c>
       <c r="B175" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C175" t="s">
         <v>27</v>
       </c>
-      <c r="D175" s="37" t="s">
-        <v>758</v>
+      <c r="D175" t="s">
+        <v>177</v>
       </c>
       <c r="I175" s="9" t="s">
-        <v>693</v>
+        <v>185</v>
+      </c>
+      <c r="M175" t="s">
+        <v>200</v>
+      </c>
+      <c r="N175" t="s">
+        <v>201</v>
+      </c>
+      <c r="O175" t="s">
+        <v>325</v>
       </c>
       <c r="P175" t="s">
-        <v>764</v>
-      </c>
-      <c r="Q175" s="1"/>
+        <v>179</v>
+      </c>
     </row>
     <row r="176" spans="1:17">
       <c r="A176" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B176" t="s">
         <v>24</v>
@@ -18272,13 +18276,13 @@
         <v>177</v>
       </c>
       <c r="I176" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="M176" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="N176" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="O176" t="s">
         <v>325</v>
@@ -18289,10 +18293,10 @@
     </row>
     <row r="177" spans="1:17">
       <c r="A177" t="s">
-        <v>167</v>
-      </c>
-      <c r="B177" t="s">
-        <v>24</v>
+        <v>161</v>
+      </c>
+      <c r="B177" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="C177" t="s">
         <v>27</v>
@@ -18301,14 +18305,10 @@
         <v>177</v>
       </c>
       <c r="I177" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="M177" t="s">
-        <v>202</v>
-      </c>
-      <c r="N177" t="s">
-        <v>203</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="M177" s="12"/>
+      <c r="N177" s="12"/>
       <c r="O177" t="s">
         <v>325</v>
       </c>
@@ -18318,10 +18318,10 @@
     </row>
     <row r="178" spans="1:17">
       <c r="A178" t="s">
-        <v>161</v>
-      </c>
-      <c r="B178" s="12" t="s">
-        <v>21</v>
+        <v>163</v>
+      </c>
+      <c r="B178" t="s">
+        <v>24</v>
       </c>
       <c r="C178" t="s">
         <v>27</v>
@@ -18330,10 +18330,14 @@
         <v>177</v>
       </c>
       <c r="I178" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="M178" s="12"/>
-      <c r="N178" s="12"/>
+        <v>182</v>
+      </c>
+      <c r="M178" t="s">
+        <v>196</v>
+      </c>
+      <c r="N178" t="s">
+        <v>197</v>
+      </c>
       <c r="O178" t="s">
         <v>325</v>
       </c>
@@ -18343,7 +18347,7 @@
     </row>
     <row r="179" spans="1:17">
       <c r="A179" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B179" t="s">
         <v>24</v>
@@ -18354,14 +18358,17 @@
       <c r="D179" t="s">
         <v>177</v>
       </c>
+      <c r="G179" t="s">
+        <v>475</v>
+      </c>
       <c r="I179" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M179" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="N179" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="O179" t="s">
         <v>325</v>
@@ -18372,29 +18379,22 @@
     </row>
     <row r="180" spans="1:17">
       <c r="A180" t="s">
-        <v>164</v>
-      </c>
-      <c r="B180" t="s">
-        <v>24</v>
+        <v>168</v>
+      </c>
+      <c r="B180" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="C180" t="s">
         <v>27</v>
       </c>
       <c r="D180" t="s">
-        <v>177</v>
-      </c>
-      <c r="G180" t="s">
-        <v>475</v>
+        <v>178</v>
       </c>
       <c r="I180" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="M180" t="s">
-        <v>198</v>
-      </c>
-      <c r="N180" t="s">
-        <v>199</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="M180" s="12"/>
+      <c r="N180" s="12"/>
       <c r="O180" t="s">
         <v>325</v>
       </c>
@@ -18404,10 +18404,10 @@
     </row>
     <row r="181" spans="1:17">
       <c r="A181" t="s">
-        <v>168</v>
-      </c>
-      <c r="B181" s="12" t="s">
-        <v>21</v>
+        <v>170</v>
+      </c>
+      <c r="B181" t="s">
+        <v>24</v>
       </c>
       <c r="C181" t="s">
         <v>27</v>
@@ -18416,10 +18416,14 @@
         <v>178</v>
       </c>
       <c r="I181" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="M181" s="12"/>
-      <c r="N181" s="12"/>
+        <v>189</v>
+      </c>
+      <c r="M181" t="s">
+        <v>206</v>
+      </c>
+      <c r="N181" t="s">
+        <v>205</v>
+      </c>
       <c r="O181" t="s">
         <v>325</v>
       </c>
@@ -18429,7 +18433,7 @@
     </row>
     <row r="182" spans="1:17">
       <c r="A182" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B182" t="s">
         <v>24</v>
@@ -18441,13 +18445,13 @@
         <v>178</v>
       </c>
       <c r="I182" s="9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="M182" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="N182" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="O182" t="s">
         <v>325</v>
@@ -18458,7 +18462,7 @@
     </row>
     <row r="183" spans="1:17">
       <c r="A183" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B183" t="s">
         <v>24</v>
@@ -18470,13 +18474,13 @@
         <v>178</v>
       </c>
       <c r="I183" s="9" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="M183" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="N183" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="O183" t="s">
         <v>325</v>
@@ -18487,7 +18491,7 @@
     </row>
     <row r="184" spans="1:17">
       <c r="A184" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B184" t="s">
         <v>24</v>
@@ -18499,13 +18503,13 @@
         <v>178</v>
       </c>
       <c r="I184" s="9" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="M184" t="s">
-        <v>211</v>
+        <v>563</v>
       </c>
       <c r="N184" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="O184" t="s">
         <v>325</v>
@@ -18516,36 +18520,27 @@
     </row>
     <row r="185" spans="1:17">
       <c r="A185" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
       <c r="B185" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C185" t="s">
         <v>27</v>
       </c>
       <c r="D185" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
       <c r="I185" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="M185" t="s">
-        <v>563</v>
-      </c>
-      <c r="N185" t="s">
-        <v>213</v>
-      </c>
-      <c r="O185" t="s">
-        <v>325</v>
+        <v>228</v>
       </c>
       <c r="P185" t="s">
-        <v>179</v>
+        <v>517</v>
       </c>
     </row>
     <row r="186" spans="1:17">
       <c r="A186" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B186" t="s">
         <v>21</v>
@@ -18554,10 +18549,10 @@
         <v>27</v>
       </c>
       <c r="D186" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I186" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="P186" t="s">
         <v>517</v>
@@ -18565,7 +18560,7 @@
     </row>
     <row r="187" spans="1:17">
       <c r="A187" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B187" t="s">
         <v>21</v>
@@ -18574,10 +18569,10 @@
         <v>27</v>
       </c>
       <c r="D187" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I187" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="P187" t="s">
         <v>517</v>
@@ -18585,7 +18580,7 @@
     </row>
     <row r="188" spans="1:17">
       <c r="A188" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B188" t="s">
         <v>21</v>
@@ -18594,10 +18589,10 @@
         <v>27</v>
       </c>
       <c r="D188" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I188" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P188" t="s">
         <v>517</v>
@@ -18605,7 +18600,7 @@
     </row>
     <row r="189" spans="1:17">
       <c r="A189" t="s">
-        <v>218</v>
+        <v>841</v>
       </c>
       <c r="B189" t="s">
         <v>21</v>
@@ -18614,18 +18609,19 @@
         <v>27</v>
       </c>
       <c r="D189" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I189" s="9" t="s">
-        <v>231</v>
+        <v>842</v>
       </c>
       <c r="P189" t="s">
         <v>517</v>
       </c>
+      <c r="Q189" s="15"/>
     </row>
     <row r="190" spans="1:17">
       <c r="A190" t="s">
-        <v>841</v>
+        <v>219</v>
       </c>
       <c r="B190" t="s">
         <v>21</v>
@@ -18637,16 +18633,15 @@
         <v>226</v>
       </c>
       <c r="I190" s="9" t="s">
-        <v>842</v>
+        <v>232</v>
       </c>
       <c r="P190" t="s">
         <v>517</v>
       </c>
-      <c r="Q190" s="15"/>
     </row>
     <row r="191" spans="1:17">
       <c r="A191" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B191" t="s">
         <v>21</v>
@@ -18658,7 +18653,7 @@
         <v>226</v>
       </c>
       <c r="I191" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="P191" t="s">
         <v>517</v>
@@ -18666,7 +18661,7 @@
     </row>
     <row r="192" spans="1:17">
       <c r="A192" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B192" t="s">
         <v>21</v>
@@ -18678,7 +18673,7 @@
         <v>226</v>
       </c>
       <c r="I192" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P192" t="s">
         <v>517</v>
@@ -18686,42 +18681,34 @@
     </row>
     <row r="193" spans="1:17">
       <c r="A193" t="s">
-        <v>221</v>
+        <v>645</v>
       </c>
       <c r="B193" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C193" t="s">
         <v>27</v>
       </c>
-      <c r="D193" t="s">
-        <v>226</v>
+      <c r="D193" s="37" t="s">
+        <v>806</v>
+      </c>
+      <c r="H193" t="s">
+        <v>807</v>
       </c>
       <c r="I193" s="9" t="s">
-        <v>234</v>
+        <v>704</v>
       </c>
       <c r="P193" t="s">
-        <v>517</v>
-      </c>
+        <v>812</v>
+      </c>
+      <c r="Q193" s="1"/>
     </row>
     <row r="194" spans="1:17">
-      <c r="A194" t="s">
-        <v>645</v>
-      </c>
-      <c r="B194" t="s">
-        <v>23</v>
-      </c>
-      <c r="C194" t="s">
-        <v>27</v>
-      </c>
-      <c r="D194" s="37" t="s">
-        <v>806</v>
-      </c>
       <c r="H194" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="I194" s="9" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="P194" t="s">
         <v>812</v>
@@ -18730,10 +18717,10 @@
     </row>
     <row r="195" spans="1:17">
       <c r="H195" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="I195" s="9" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="P195" t="s">
         <v>812</v>
@@ -18742,10 +18729,10 @@
     </row>
     <row r="196" spans="1:17">
       <c r="H196" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="I196" s="9" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="P196" t="s">
         <v>812</v>
@@ -18754,10 +18741,10 @@
     </row>
     <row r="197" spans="1:17">
       <c r="H197" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="I197" s="9" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="P197" t="s">
         <v>812</v>
@@ -18765,20 +18752,29 @@
       <c r="Q197" s="1"/>
     </row>
     <row r="198" spans="1:17">
-      <c r="H198" t="s">
-        <v>811</v>
+      <c r="A198" t="s">
+        <v>585</v>
+      </c>
+      <c r="B198" t="s">
+        <v>21</v>
+      </c>
+      <c r="C198" t="s">
+        <v>27</v>
+      </c>
+      <c r="D198" s="37" t="s">
+        <v>709</v>
       </c>
       <c r="I198" s="9" t="s">
-        <v>708</v>
+        <v>681</v>
       </c>
       <c r="P198" t="s">
-        <v>812</v>
+        <v>829</v>
       </c>
       <c r="Q198" s="1"/>
     </row>
     <row r="199" spans="1:17">
       <c r="A199" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B199" t="s">
         <v>21</v>
@@ -18787,19 +18783,19 @@
         <v>27</v>
       </c>
       <c r="D199" s="37" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="I199" s="9" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="P199" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="Q199" s="1"/>
     </row>
     <row r="200" spans="1:17">
       <c r="A200" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B200" t="s">
         <v>21</v>
@@ -18808,19 +18804,19 @@
         <v>27</v>
       </c>
       <c r="D200" s="37" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I200" s="9" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="P200" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="Q200" s="1"/>
     </row>
     <row r="201" spans="1:17">
       <c r="A201" t="s">
-        <v>586</v>
+        <v>813</v>
       </c>
       <c r="B201" t="s">
         <v>21</v>
@@ -18828,20 +18824,20 @@
       <c r="C201" t="s">
         <v>27</v>
       </c>
-      <c r="D201" s="37" t="s">
-        <v>710</v>
+      <c r="D201" t="s">
+        <v>380</v>
       </c>
       <c r="I201" s="9" t="s">
-        <v>682</v>
+        <v>814</v>
       </c>
       <c r="P201" t="s">
-        <v>830</v>
+        <v>382</v>
       </c>
       <c r="Q201" s="1"/>
     </row>
     <row r="202" spans="1:17">
       <c r="A202" t="s">
-        <v>813</v>
+        <v>381</v>
       </c>
       <c r="B202" t="s">
         <v>21</v>
@@ -18853,16 +18849,15 @@
         <v>380</v>
       </c>
       <c r="I202" s="9" t="s">
-        <v>814</v>
+        <v>379</v>
       </c>
       <c r="P202" t="s">
         <v>382</v>
       </c>
-      <c r="Q202" s="1"/>
     </row>
     <row r="203" spans="1:17">
       <c r="A203" t="s">
-        <v>381</v>
+        <v>331</v>
       </c>
       <c r="B203" t="s">
         <v>21</v>
@@ -18871,18 +18866,18 @@
         <v>27</v>
       </c>
       <c r="D203" t="s">
-        <v>380</v>
+        <v>341</v>
       </c>
       <c r="I203" s="9" t="s">
-        <v>379</v>
+        <v>351</v>
       </c>
       <c r="P203" t="s">
-        <v>382</v>
+        <v>540</v>
       </c>
     </row>
     <row r="204" spans="1:17">
       <c r="A204" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B204" t="s">
         <v>21</v>
@@ -18891,10 +18886,10 @@
         <v>27</v>
       </c>
       <c r="D204" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I204" s="9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="P204" t="s">
         <v>540</v>
@@ -18902,7 +18897,7 @@
     </row>
     <row r="205" spans="1:17">
       <c r="A205" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B205" t="s">
         <v>21</v>
@@ -18911,10 +18906,10 @@
         <v>27</v>
       </c>
       <c r="D205" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="I205" s="9" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="P205" t="s">
         <v>540</v>
@@ -18922,7 +18917,7 @@
     </row>
     <row r="206" spans="1:17">
       <c r="A206" t="s">
-        <v>335</v>
+        <v>594</v>
       </c>
       <c r="B206" t="s">
         <v>21</v>
@@ -18930,19 +18925,20 @@
       <c r="C206" t="s">
         <v>27</v>
       </c>
-      <c r="D206" t="s">
-        <v>345</v>
+      <c r="D206" s="37" t="s">
+        <v>716</v>
       </c>
       <c r="I206" s="9" t="s">
-        <v>355</v>
+        <v>690</v>
       </c>
       <c r="P206" t="s">
-        <v>540</v>
-      </c>
+        <v>757</v>
+      </c>
+      <c r="Q206" s="1"/>
     </row>
     <row r="207" spans="1:17">
       <c r="A207" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B207" t="s">
         <v>21</v>
@@ -18951,19 +18947,19 @@
         <v>27</v>
       </c>
       <c r="D207" s="37" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="I207" s="9" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="P207" t="s">
-        <v>757</v>
+        <v>763</v>
       </c>
       <c r="Q207" s="1"/>
     </row>
     <row r="208" spans="1:17">
       <c r="A208" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B208" t="s">
         <v>21</v>
@@ -18972,10 +18968,10 @@
         <v>27</v>
       </c>
       <c r="D208" s="37" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="I208" s="9" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="P208" t="s">
         <v>763</v>
@@ -18984,7 +18980,7 @@
     </row>
     <row r="209" spans="1:17">
       <c r="A209" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B209" t="s">
         <v>21</v>
@@ -18993,19 +18989,19 @@
         <v>27</v>
       </c>
       <c r="D209" s="37" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="I209" s="9" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="P209" t="s">
-        <v>763</v>
+        <v>832</v>
       </c>
       <c r="Q209" s="1"/>
     </row>
     <row r="210" spans="1:17">
       <c r="A210" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B210" t="s">
         <v>21</v>
@@ -19017,7 +19013,7 @@
         <v>711</v>
       </c>
       <c r="I210" s="9" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="P210" t="s">
         <v>832</v>
@@ -19026,7 +19022,7 @@
     </row>
     <row r="211" spans="1:17">
       <c r="A211" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="B211" t="s">
         <v>21</v>
@@ -19035,19 +19031,19 @@
         <v>27</v>
       </c>
       <c r="D211" s="37" t="s">
-        <v>711</v>
+        <v>759</v>
       </c>
       <c r="I211" s="9" t="s">
-        <v>686</v>
+        <v>694</v>
       </c>
       <c r="P211" t="s">
-        <v>832</v>
+        <v>357</v>
       </c>
       <c r="Q211" s="1"/>
     </row>
     <row r="212" spans="1:17">
       <c r="A212" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B212" t="s">
         <v>21</v>
@@ -19056,10 +19052,10 @@
         <v>27</v>
       </c>
       <c r="D212" s="37" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="I212" s="9" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="P212" t="s">
         <v>357</v>
@@ -19068,7 +19064,7 @@
     </row>
     <row r="213" spans="1:17">
       <c r="A213" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="B213" t="s">
         <v>21</v>
@@ -19077,10 +19073,10 @@
         <v>27</v>
       </c>
       <c r="D213" s="37" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="I213" s="9" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="P213" t="s">
         <v>357</v>
@@ -19089,7 +19085,7 @@
     </row>
     <row r="214" spans="1:17">
       <c r="A214" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B214" t="s">
         <v>21</v>
@@ -19098,10 +19094,10 @@
         <v>27</v>
       </c>
       <c r="D214" s="37" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="I214" s="9" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P214" t="s">
         <v>357</v>
@@ -19110,7 +19106,7 @@
     </row>
     <row r="215" spans="1:17">
       <c r="A215" t="s">
-        <v>600</v>
+        <v>333</v>
       </c>
       <c r="B215" t="s">
         <v>21</v>
@@ -19118,20 +19114,19 @@
       <c r="C215" t="s">
         <v>27</v>
       </c>
-      <c r="D215" s="37" t="s">
-        <v>761</v>
+      <c r="D215" t="s">
+        <v>343</v>
       </c>
       <c r="I215" s="9" t="s">
-        <v>696</v>
+        <v>353</v>
       </c>
       <c r="P215" t="s">
         <v>357</v>
       </c>
-      <c r="Q215" s="1"/>
     </row>
     <row r="216" spans="1:17">
       <c r="A216" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B216" t="s">
         <v>21</v>
@@ -19140,10 +19135,10 @@
         <v>27</v>
       </c>
       <c r="D216" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="I216" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="P216" t="s">
         <v>357</v>
@@ -19151,7 +19146,7 @@
     </row>
     <row r="217" spans="1:17">
       <c r="A217" t="s">
-        <v>334</v>
+        <v>252</v>
       </c>
       <c r="B217" t="s">
         <v>21</v>
@@ -19160,18 +19155,18 @@
         <v>27</v>
       </c>
       <c r="D217" t="s">
-        <v>344</v>
+        <v>294</v>
       </c>
       <c r="I217" s="9" t="s">
-        <v>354</v>
+        <v>273</v>
       </c>
       <c r="P217" t="s">
-        <v>357</v>
+        <v>539</v>
       </c>
     </row>
     <row r="218" spans="1:17">
       <c r="A218" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B218" t="s">
         <v>21</v>
@@ -19183,7 +19178,7 @@
         <v>294</v>
       </c>
       <c r="I218" s="9" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P218" t="s">
         <v>539</v>
@@ -19191,7 +19186,7 @@
     </row>
     <row r="219" spans="1:17">
       <c r="A219" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B219" t="s">
         <v>21</v>
@@ -19203,7 +19198,7 @@
         <v>294</v>
       </c>
       <c r="I219" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="P219" t="s">
         <v>539</v>
@@ -19211,7 +19206,7 @@
     </row>
     <row r="220" spans="1:17">
       <c r="A220" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B220" t="s">
         <v>21</v>
@@ -19223,7 +19218,7 @@
         <v>294</v>
       </c>
       <c r="I220" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="P220" t="s">
         <v>539</v>
@@ -19231,7 +19226,7 @@
     </row>
     <row r="221" spans="1:17">
       <c r="A221" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B221" t="s">
         <v>21</v>
@@ -19243,7 +19238,7 @@
         <v>294</v>
       </c>
       <c r="I221" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="P221" t="s">
         <v>539</v>
@@ -19251,7 +19246,7 @@
     </row>
     <row r="222" spans="1:17">
       <c r="A222" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B222" t="s">
         <v>21</v>
@@ -19263,7 +19258,7 @@
         <v>294</v>
       </c>
       <c r="I222" s="9" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="P222" t="s">
         <v>539</v>
@@ -19271,7 +19266,7 @@
     </row>
     <row r="223" spans="1:17">
       <c r="A223" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B223" t="s">
         <v>21</v>
@@ -19283,7 +19278,7 @@
         <v>294</v>
       </c>
       <c r="I223" s="9" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="P223" t="s">
         <v>539</v>
@@ -19291,7 +19286,7 @@
     </row>
     <row r="224" spans="1:17">
       <c r="A224" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B224" t="s">
         <v>21</v>
@@ -19303,7 +19298,7 @@
         <v>294</v>
       </c>
       <c r="I224" s="9" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="P224" t="s">
         <v>539</v>
@@ -19311,7 +19306,7 @@
     </row>
     <row r="225" spans="1:16">
       <c r="A225" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B225" t="s">
         <v>21</v>
@@ -19323,7 +19318,7 @@
         <v>294</v>
       </c>
       <c r="I225" s="9" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="P225" t="s">
         <v>539</v>
@@ -19331,7 +19326,7 @@
     </row>
     <row r="226" spans="1:16">
       <c r="A226" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B226" t="s">
         <v>21</v>
@@ -19343,7 +19338,7 @@
         <v>294</v>
       </c>
       <c r="I226" s="9" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="P226" t="s">
         <v>539</v>
@@ -19351,7 +19346,7 @@
     </row>
     <row r="227" spans="1:16">
       <c r="A227" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B227" t="s">
         <v>21</v>
@@ -19363,7 +19358,7 @@
         <v>294</v>
       </c>
       <c r="I227" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P227" t="s">
         <v>539</v>
@@ -19371,7 +19366,7 @@
     </row>
     <row r="228" spans="1:16">
       <c r="A228" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B228" t="s">
         <v>21</v>
@@ -19383,7 +19378,7 @@
         <v>294</v>
       </c>
       <c r="I228" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="P228" t="s">
         <v>539</v>
@@ -19391,7 +19386,7 @@
     </row>
     <row r="229" spans="1:16">
       <c r="A229" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B229" t="s">
         <v>21</v>
@@ -19403,7 +19398,7 @@
         <v>294</v>
       </c>
       <c r="I229" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="P229" t="s">
         <v>539</v>
@@ -19411,7 +19406,7 @@
     </row>
     <row r="230" spans="1:16">
       <c r="A230" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B230" t="s">
         <v>21</v>
@@ -19423,7 +19418,7 @@
         <v>294</v>
       </c>
       <c r="I230" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="P230" t="s">
         <v>539</v>
@@ -19431,7 +19426,7 @@
     </row>
     <row r="231" spans="1:16">
       <c r="A231" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B231" t="s">
         <v>21</v>
@@ -19443,7 +19438,7 @@
         <v>294</v>
       </c>
       <c r="I231" s="9" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="P231" t="s">
         <v>539</v>
@@ -19451,7 +19446,7 @@
     </row>
     <row r="232" spans="1:16">
       <c r="A232" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B232" t="s">
         <v>21</v>
@@ -19463,7 +19458,7 @@
         <v>294</v>
       </c>
       <c r="I232" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="P232" t="s">
         <v>539</v>
@@ -19471,7 +19466,7 @@
     </row>
     <row r="233" spans="1:16">
       <c r="A233" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B233" t="s">
         <v>21</v>
@@ -19483,7 +19478,7 @@
         <v>294</v>
       </c>
       <c r="I233" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="P233" t="s">
         <v>539</v>
@@ -19491,7 +19486,7 @@
     </row>
     <row r="234" spans="1:16">
       <c r="A234" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B234" t="s">
         <v>21</v>
@@ -19503,7 +19498,7 @@
         <v>294</v>
       </c>
       <c r="I234" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="P234" t="s">
         <v>539</v>
@@ -19511,7 +19506,7 @@
     </row>
     <row r="235" spans="1:16">
       <c r="A235" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B235" t="s">
         <v>21</v>
@@ -19523,7 +19518,7 @@
         <v>294</v>
       </c>
       <c r="I235" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="P235" t="s">
         <v>539</v>
@@ -19531,7 +19526,7 @@
     </row>
     <row r="236" spans="1:16">
       <c r="A236" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B236" t="s">
         <v>21</v>
@@ -19543,7 +19538,7 @@
         <v>294</v>
       </c>
       <c r="I236" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="P236" t="s">
         <v>539</v>
@@ -19551,7 +19546,7 @@
     </row>
     <row r="237" spans="1:16">
       <c r="A237" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B237" t="s">
         <v>21</v>
@@ -19563,7 +19558,7 @@
         <v>294</v>
       </c>
       <c r="I237" s="9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="P237" t="s">
         <v>539</v>
@@ -19571,7 +19566,7 @@
     </row>
     <row r="238" spans="1:16">
       <c r="A238" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="B238" t="s">
         <v>21</v>
@@ -19580,10 +19575,10 @@
         <v>27</v>
       </c>
       <c r="D238" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="I238" s="9" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="P238" t="s">
         <v>539</v>
@@ -19591,7 +19586,7 @@
     </row>
     <row r="239" spans="1:16">
       <c r="A239" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B239" t="s">
         <v>21</v>
@@ -19603,7 +19598,7 @@
         <v>299</v>
       </c>
       <c r="I239" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="P239" t="s">
         <v>539</v>
@@ -19611,7 +19606,7 @@
     </row>
     <row r="240" spans="1:16">
       <c r="A240" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B240" t="s">
         <v>21</v>
@@ -19623,7 +19618,7 @@
         <v>299</v>
       </c>
       <c r="I240" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P240" t="s">
         <v>539</v>
@@ -19631,7 +19626,7 @@
     </row>
     <row r="241" spans="1:17">
       <c r="A241" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B241" t="s">
         <v>21</v>
@@ -19643,7 +19638,7 @@
         <v>299</v>
       </c>
       <c r="I241" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="P241" t="s">
         <v>539</v>
@@ -19651,7 +19646,7 @@
     </row>
     <row r="242" spans="1:17">
       <c r="A242" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="B242" t="s">
         <v>21</v>
@@ -19660,10 +19655,10 @@
         <v>27</v>
       </c>
       <c r="D242" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="I242" s="9" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="P242" t="s">
         <v>539</v>
@@ -19671,7 +19666,7 @@
     </row>
     <row r="243" spans="1:17">
       <c r="A243" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B243" t="s">
         <v>21</v>
@@ -19683,7 +19678,7 @@
         <v>316</v>
       </c>
       <c r="I243" s="9" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="P243" t="s">
         <v>539</v>
@@ -19691,7 +19686,7 @@
     </row>
     <row r="244" spans="1:17">
       <c r="A244" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B244" t="s">
         <v>21</v>
@@ -19703,7 +19698,7 @@
         <v>316</v>
       </c>
       <c r="I244" s="9" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="P244" t="s">
         <v>539</v>
@@ -19711,7 +19706,7 @@
     </row>
     <row r="245" spans="1:17">
       <c r="A245" t="s">
-        <v>308</v>
+        <v>584</v>
       </c>
       <c r="B245" t="s">
         <v>21</v>
@@ -19719,19 +19714,20 @@
       <c r="C245" t="s">
         <v>27</v>
       </c>
-      <c r="D245" t="s">
-        <v>316</v>
+      <c r="D245" s="37" t="s">
+        <v>709</v>
       </c>
       <c r="I245" s="9" t="s">
-        <v>314</v>
+        <v>680</v>
       </c>
       <c r="P245" t="s">
-        <v>539</v>
-      </c>
+        <v>833</v>
+      </c>
+      <c r="Q245" s="1"/>
     </row>
     <row r="246" spans="1:17">
       <c r="A246" t="s">
-        <v>584</v>
+        <v>328</v>
       </c>
       <c r="B246" t="s">
         <v>21</v>
@@ -19739,90 +19735,90 @@
       <c r="C246" t="s">
         <v>27</v>
       </c>
-      <c r="D246" s="37" t="s">
-        <v>709</v>
+      <c r="D246" t="s">
+        <v>338</v>
       </c>
       <c r="I246" s="9" t="s">
-        <v>680</v>
+        <v>348</v>
       </c>
       <c r="P246" t="s">
-        <v>833</v>
-      </c>
-      <c r="Q246" s="1"/>
+        <v>356</v>
+      </c>
     </row>
     <row r="247" spans="1:17">
       <c r="A247" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B247" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C247" t="s">
         <v>27</v>
       </c>
       <c r="D247" t="s">
-        <v>338</v>
+        <v>317</v>
+      </c>
+      <c r="G247" t="s">
+        <v>475</v>
       </c>
       <c r="I247" s="9" t="s">
-        <v>348</v>
+        <v>318</v>
+      </c>
+      <c r="M247" t="s">
+        <v>473</v>
+      </c>
+      <c r="N247" t="s">
+        <v>322</v>
+      </c>
+      <c r="O247" t="s">
+        <v>323</v>
       </c>
       <c r="P247" t="s">
-        <v>356</v>
+        <v>321</v>
       </c>
     </row>
     <row r="248" spans="1:17">
-      <c r="A248" t="s">
-        <v>319</v>
-      </c>
-      <c r="B248" t="s">
-        <v>24</v>
-      </c>
-      <c r="C248" t="s">
-        <v>27</v>
-      </c>
-      <c r="D248" t="s">
-        <v>317</v>
-      </c>
       <c r="G248" t="s">
         <v>475</v>
       </c>
-      <c r="I248" s="9" t="s">
-        <v>318</v>
-      </c>
+      <c r="I248" s="9"/>
       <c r="M248" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="N248" t="s">
-        <v>322</v>
+        <v>472</v>
       </c>
       <c r="O248" t="s">
-        <v>323</v>
+        <v>471</v>
       </c>
       <c r="P248" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="249" spans="1:17">
-      <c r="G249" t="s">
-        <v>475</v>
-      </c>
-      <c r="I249" s="9"/>
-      <c r="M249" t="s">
-        <v>474</v>
-      </c>
-      <c r="N249" t="s">
-        <v>472</v>
-      </c>
-      <c r="O249" t="s">
-        <v>471</v>
+      <c r="A249" t="s">
+        <v>644</v>
+      </c>
+      <c r="B249" t="s">
+        <v>21</v>
+      </c>
+      <c r="C249" t="s">
+        <v>27</v>
+      </c>
+      <c r="D249" s="37" t="s">
+        <v>805</v>
+      </c>
+      <c r="I249" s="9" t="s">
+        <v>703</v>
       </c>
       <c r="P249" t="s">
-        <v>320</v>
-      </c>
+        <v>835</v>
+      </c>
+      <c r="Q249" s="1"/>
     </row>
     <row r="250" spans="1:17">
       <c r="A250" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B250" t="s">
         <v>21</v>
@@ -19831,19 +19827,19 @@
         <v>27</v>
       </c>
       <c r="D250" s="37" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I250" s="9" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="P250" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="Q250" s="1"/>
     </row>
     <row r="251" spans="1:17">
       <c r="A251" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B251" t="s">
         <v>21</v>
@@ -19852,36 +19848,15 @@
         <v>27</v>
       </c>
       <c r="D251" s="37" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="I251" s="9" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="P251" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="Q251" s="1"/>
-    </row>
-    <row r="252" spans="1:17">
-      <c r="A252" t="s">
-        <v>642</v>
-      </c>
-      <c r="B252" t="s">
-        <v>21</v>
-      </c>
-      <c r="C252" t="s">
-        <v>27</v>
-      </c>
-      <c r="D252" s="37" t="s">
-        <v>803</v>
-      </c>
-      <c r="I252" s="9" t="s">
-        <v>701</v>
-      </c>
-      <c r="P252" t="s">
-        <v>834</v>
-      </c>
-      <c r="Q252" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -19892,45 +19867,45 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C163:C165 C167 C191:C193 C161 C176:C189 C169 C151:C159 C203:C206 C174 C149 C216:C245 C247:C248">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C162:C164 C166 C190:C192 C160 C175:C188 C168 C150:C158 C202:C205 C173 C148 C215:C244 C246:C247">
       <formula1>$AC$1:$AC$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B163:B165 B167 B191:B193 B161 B176:B189 B169 B151:B159 B203:B206 B174 B149 B216:B245 B247:B248">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B162:B164 B166 B190:B192 B160 B175:B188 B168 B150:B158 B202:B205 B173 B148 B215:B244 B246:B247">
       <formula1>$AB$1:$AB$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B132:B135 B138:B148 B118:B130 B3:B14 B76 B84 B79 B16:B33 B105:B113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B131:B134 B137:B147 B117:B129 B3:B14 B75 B83 B78 B16:B33 B104:B112">
       <formula1>$AB$1:$AB$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C132:C135 C138:C148 C118:C130 C3:C14 C76 C84 C79 C16:C33 C105:C113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C131:C134 C137:C147 C117:C129 C3:C14 C75 C83 C78 C16:C33 C104:C112">
       <formula1>$AC$1:$AC$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B166 B168 B170 B160 B162 B202 B190 B136:B137 B131 B15 B194 B77:B78 B80:B83 B85:B104">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B165 B167 B169 B159 B161 B201 B189 B135:B136 B130 B15 B193 B76:B77 B79:B82 B84:B103">
       <formula1>$AB$1:$AB$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C166 C168 C170 C160 C162 C202 C190 C136:C137 C131 C15 C194 C77:C78 C80:C83 C85:C104">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C165 C167 C169 C159 C161 C201 C189 C135:C136 C130 C15 C193 C76:C77 C79:C82 C84:C103">
       <formula1>$AC$1:$AC$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B171:B173 B175 B212:B215 B207:B209 B250:B252 B75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B170:B172 B174 B211:B214 B206:B208 B249:B251 B74">
       <formula1>$AB$1:$AB$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C171:C173 C175 C212:C215 C207:C209 C250:C252 C75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C170:C172 C174 C211:C214 C206:C208 C249:C251 C74">
       <formula1>$AC$1:$AC$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B150 B246 B210:B211 B199:B201">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B149 B245 B209:B210 B198:B200">
       <formula1>$AB$1:$AB$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C150 C246 C210:C211 C199:C201">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C149 C245 C209:C210 C198:C200">
       <formula1>$AC$1:$AC$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C34:C55 C56:C74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C34:C73">
       <formula1>$AC$1:$AC$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34:B55 B56:B74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34:B73">
       <formula1>$AB$1:$AB$9</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D109" r:id="rId1"/>
+    <hyperlink ref="D108" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>